<commit_message>
Divide npc and Player. Add PlayerAttributes Add Item , SKill , Equipment, Pet , Achievement structure Add IUsable, IDissolvable, ICombinable, IEquipable, IEnhancable
</commit_message>
<xml_diff>
--- a/Assets/Scripts/1.Abilities/Effects/Resources/Documents/Ability/NpcTraits.xlsx
+++ b/Assets/Scripts/1.Abilities/Effects/Resources/Documents/Ability/NpcTraits.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\myWorks\Unity-BolierPlate-Codes\Assets\Scripts\1.Abilities\Effects\Resources\Documents\Ability\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\BackUp 2023-0324\Unity Portfolios\BoilerPlate\BP\Assets\Scripts\1.Abilities\Effects\Resources\Documents\Ability\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EB1BCC4-B33D-4B8A-AE73-90E7FEC67644}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7783F36A-ACD9-4613-8017-EB0245E1E1BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="2" xr2:uid="{4F09BE30-3FCF-46F0-A93C-3CEDA836A106}"/>
+    <workbookView xWindow="11430" yWindow="7140" windowWidth="24900" windowHeight="11860" xr2:uid="{4F09BE30-3FCF-46F0-A93C-3CEDA836A106}"/>
   </bookViews>
   <sheets>
     <sheet name="Attribute" sheetId="5" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="69">
   <si>
     <t>Name</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -303,6 +303,14 @@
   </si>
   <si>
     <t>LootMythItems</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Places</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MotivationSkills</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -670,21 +678,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FC57950A-9E23-4278-A211-D37973D388E6}">
-  <dimension ref="A1:N11"/>
+  <dimension ref="A1:O11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K1" sqref="K1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M8" sqref="M8:O8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="6.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
     <col min="3" max="6" width="11" customWidth="1"/>
-    <col min="7" max="9" width="13.375" customWidth="1"/>
+    <col min="7" max="9" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -715,75 +723,81 @@
       <c r="J1" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="K1" t="s">
+        <v>68</v>
+      </c>
+      <c r="L1" t="s">
+        <v>67</v>
+      </c>
+      <c r="M1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="M1" s="1"/>
       <c r="N1" s="1"/>
-    </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="L2" s="1"/>
+      <c r="O1" s="1"/>
+    </row>
+    <row r="2" spans="1:15" x14ac:dyDescent="0.45">
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="L3" s="1"/>
+      <c r="O2" s="1"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.45">
       <c r="M3" s="1"/>
       <c r="N3" s="1"/>
-    </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="L4" s="1"/>
+      <c r="O3" s="1"/>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.45">
       <c r="M4" s="1"/>
       <c r="N4" s="1"/>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="L5" s="1"/>
+      <c r="O4" s="1"/>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.45">
       <c r="M5" s="1"/>
       <c r="N5" s="1"/>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="L6" s="1"/>
+      <c r="O5" s="1"/>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.45">
       <c r="M6" s="1"/>
       <c r="N6" s="1"/>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="L7" s="1"/>
+      <c r="O6" s="1"/>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.45">
       <c r="M7" s="1"/>
       <c r="N7" s="1"/>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="L8" s="1"/>
+      <c r="O7" s="1"/>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.45">
       <c r="M8" s="1"/>
       <c r="N8" s="1"/>
-    </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="L9" s="1"/>
+      <c r="O8" s="1"/>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.45">
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="L10" s="1"/>
+      <c r="O9" s="1"/>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.45">
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
-      <c r="L11" s="1"/>
+      <c r="O10" s="1"/>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.45">
       <c r="M11" s="1"/>
       <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
     </row>
   </sheetData>
   <mergeCells count="11">
-    <mergeCell ref="L7:N7"/>
-    <mergeCell ref="L8:N8"/>
-    <mergeCell ref="L9:N9"/>
-    <mergeCell ref="L10:N10"/>
-    <mergeCell ref="L11:N11"/>
-    <mergeCell ref="L6:N6"/>
-    <mergeCell ref="L1:N1"/>
-    <mergeCell ref="L2:N2"/>
-    <mergeCell ref="L3:N3"/>
-    <mergeCell ref="L4:N4"/>
-    <mergeCell ref="L5:N5"/>
+    <mergeCell ref="M6:O6"/>
+    <mergeCell ref="M1:O1"/>
+    <mergeCell ref="M2:O2"/>
+    <mergeCell ref="M3:O3"/>
+    <mergeCell ref="M4:O4"/>
+    <mergeCell ref="M5:O5"/>
+    <mergeCell ref="M7:O7"/>
+    <mergeCell ref="M8:O8"/>
+    <mergeCell ref="M9:O9"/>
+    <mergeCell ref="M10:O10"/>
+    <mergeCell ref="M11:O11"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -798,9 +812,9 @@
       <selection activeCell="R24" sqref="R24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>4</v>
       </c>
@@ -811,7 +825,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A2" t="s">
         <v>12</v>
       </c>
@@ -822,7 +836,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>13</v>
       </c>
@@ -833,7 +847,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>14</v>
       </c>
@@ -844,7 +858,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>15</v>
       </c>
@@ -855,7 +869,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
         <v>30</v>
       </c>
@@ -866,7 +880,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>49</v>
       </c>
@@ -877,7 +891,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>17</v>
       </c>
@@ -888,7 +902,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>18</v>
       </c>
@@ -896,7 +910,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>19</v>
       </c>
@@ -904,7 +918,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>20</v>
       </c>
@@ -912,7 +926,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>21</v>
       </c>
@@ -920,7 +934,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -928,7 +942,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>50</v>
       </c>
@@ -936,7 +950,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>51</v>
       </c>
@@ -944,7 +958,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>52</v>
       </c>
@@ -952,27 +966,27 @@
         <v>44</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B17" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="18" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B18" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="19" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B19" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B20" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.45">
       <c r="B21" t="s">
         <v>48</v>
       </c>
@@ -988,19 +1002,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72042D48-B804-41C9-A2ED-6F32641A601D}">
   <dimension ref="A1:O1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L21" sqref="L21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N1" sqref="N1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="17" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="6.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="11" bestFit="1" customWidth="1"/>
     <col min="3" max="4" width="11" customWidth="1"/>
-    <col min="5" max="10" width="13.375" customWidth="1"/>
+    <col min="5" max="10" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>

</xml_diff>